<commit_message>
Closed out sprint 2, started sprint 3
</commit_message>
<xml_diff>
--- a/project/Sprint02.xlsx
+++ b/project/Sprint02.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" tabRatio="725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" tabRatio="725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,8 @@
     <t>Totals</t>
   </si>
   <si>
-    <t>Lots of carry over from sprint 1</t>
+    <t>Lots of carry over from sprint 1
+Meeting over weekend let us accomplish much more work. Find it hard to meet with busy schedules during week.</t>
   </si>
 </sst>
 </file>
@@ -505,25 +506,25 @@
                   <c:v>Initial Estimate of Efforts</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/2/2016</c:v>
+                  <c:v>2/9/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/3/2016</c:v>
+                  <c:v>2/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2/4/2016</c:v>
+                  <c:v>2/11/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2/5/2016</c:v>
+                  <c:v>2/12/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2/6/2016</c:v>
+                  <c:v>2/13/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2/7/2016</c:v>
+                  <c:v>2/14/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2/8/2016</c:v>
+                  <c:v>2/15/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -547,16 +548,16 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -603,25 +604,25 @@
                   <c:v>Initial Estimate of Efforts</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/2/2016</c:v>
+                  <c:v>2/9/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/3/2016</c:v>
+                  <c:v>2/10/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2/4/2016</c:v>
+                  <c:v>2/11/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2/5/2016</c:v>
+                  <c:v>2/12/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2/6/2016</c:v>
+                  <c:v>2/13/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2/7/2016</c:v>
+                  <c:v>2/14/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2/8/2016</c:v>
+                  <c:v>2/15/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1743,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A2" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,25 +1777,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="7">
-        <v>42402</v>
+        <v>42409</v>
       </c>
       <c r="F1" s="7">
-        <v>42403</v>
+        <v>42410</v>
       </c>
       <c r="G1" s="7">
-        <v>42404</v>
+        <v>42411</v>
       </c>
       <c r="H1" s="7">
-        <v>42405</v>
+        <v>42412</v>
       </c>
       <c r="I1" s="7">
-        <v>42406</v>
+        <v>42413</v>
       </c>
       <c r="J1" s="7">
-        <v>42407</v>
+        <v>42414</v>
       </c>
       <c r="K1" s="7">
-        <v>42408</v>
+        <v>42415</v>
       </c>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -1828,19 +1829,19 @@
       </c>
       <c r="H2" s="25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>19.5</v>
       </c>
       <c r="I2" s="25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>19.5</v>
       </c>
       <c r="J2" s="25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>13.5</v>
       </c>
       <c r="K2" s="25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1899,7 +1900,7 @@
         <v>0.5</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E18" si="2">D4</f>
+        <f t="shared" ref="E4:E5" si="2">D4</f>
         <v>0.5</v>
       </c>
       <c r="F4">
@@ -2108,12 +2109,11 @@
         <v>4</v>
       </c>
       <c r="J8">
-        <f t="shared" si="14"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2234,12 +2234,11 @@
         <v>4</v>
       </c>
       <c r="J11">
-        <f t="shared" si="14"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2394,20 +2393,18 @@
         <v>2</v>
       </c>
       <c r="H15">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I15">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="J15">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K15">
-        <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2436,20 +2433,18 @@
         <v>2</v>
       </c>
       <c r="H16">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I16">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="J16">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K16">
-        <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2478,20 +2473,19 @@
         <v>2</v>
       </c>
       <c r="H17">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I17">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="J17">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K17">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2532,8 +2526,7 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2592,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>